<commit_message>
I made improvement in the code.
</commit_message>
<xml_diff>
--- a/2023-10-01monthly_file.xlsx
+++ b/2023-10-01monthly_file.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="35">
   <si>
     <t>day</t>
   </si>
@@ -101,6 +101,24 @@
   </si>
   <si>
     <t>16:37:17</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>2023-10-31</t>
+  </si>
+  <si>
+    <t>17:54:37</t>
+  </si>
+  <si>
+    <t>18:02:14</t>
+  </si>
+  <si>
+    <t>18:05:50</t>
+  </si>
+  <si>
+    <t>18:06:12</t>
   </si>
 </sst>
 </file>
@@ -432,7 +450,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -594,6 +612,110 @@
         <v>15</v>
       </c>
     </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>